<commit_message>
Changed direction column name
</commit_message>
<xml_diff>
--- a/Skyze_Indicators_Library/Unit_Test/Test_Data/Crosses/Test-Calcs-Crosses-bitcoin.xlsx
+++ b/Skyze_Indicators_Library/Unit_Test/Test_Data/Crosses/Test-Calcs-Crosses-bitcoin.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelnew/Dropbox/Aptana_Workspace/Skyze/Unit_Test/Test_Data/Indicators/Crosses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelnew/Dropbox/Aptana_Workspace/Skyze/Skyze_Indicators_Library/Unit_Test/Test_Data/Crosses/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,9 +54,6 @@
     <t>Vol</t>
   </si>
   <si>
-    <t>DIRECTION</t>
-  </si>
-  <si>
     <t>TGT_DIFF</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>MarketCap</t>
+  </si>
+  <si>
+    <t>Crosses_direction</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,22 +514,22 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -60624,7 +60624,7 @@
         <v>41816500000</v>
       </c>
       <c r="H1553" s="5">
-        <f t="shared" ref="H1553:H1616" si="98">AVERAGE(E1538:E1552)</f>
+        <f t="shared" ref="H1553:H1587" si="98">AVERAGE(E1538:E1552)</f>
         <v>2441.7433333333329</v>
       </c>
       <c r="I1553" s="5">
@@ -61213,7 +61213,7 @@
         <v>2997.2526666666668</v>
       </c>
       <c r="I1568" s="5">
-        <f t="shared" ref="I1568:I1631" si="99">AVERAGE(E1538:E1567)</f>
+        <f t="shared" ref="I1568:I1587" si="99">AVERAGE(E1538:E1567)</f>
         <v>2719.498</v>
       </c>
       <c r="J1568" s="7">

</xml_diff>